<commit_message>
aggiornata foto e rimozioni vincoli superflui
</commit_message>
<xml_diff>
--- a/EVRP3/path.xlsx
+++ b/EVRP3/path.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stela\Desktop\EVRP\EVRP3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCACF404-5B58-429B-8076-41AB13E4FC6D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85D6E6EB-49C7-4BDA-819E-B2F81068E318}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-7770" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -712,7 +712,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A9EEE833-2D8A-46E5-98F9-B9F4B814318D}" type="CELLRANGE">
+                    <a:fld id="{93603EDA-3F29-4082-87C4-C0DBE682B350}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[INTERVALLOCELLE]</a:t>
@@ -744,8 +744,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{43C4B237-1822-417E-BCB6-42B8AE00E568}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{77BDFA7E-B930-42CE-8B27-56F3FFBFCB53}" type="CELLRANGE">
+                      <a:rPr lang="it-IT"/>
                       <a:pPr/>
                       <a:t>[INTERVALLOCELLE]</a:t>
                     </a:fld>
@@ -762,6 +762,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -782,7 +783,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{30CF4218-5BAF-41CD-9646-3FA843F4B233}" type="CELLRANGE">
+                    <a:fld id="{57955B54-F7E3-4A62-9E52-52802C9B49C5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[INTERVALLOCELLE]</a:t>
@@ -1044,7 +1045,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FB65E376-2B64-4D90-833E-CBD86F595C56}" type="CELLRANGE">
+                    <a:fld id="{F9E7246A-32A6-4E18-9C14-82D5681802E1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[INTERVALLOCELLE]</a:t>
@@ -1082,7 +1083,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F7B36690-8ED2-441A-981F-059B43665FB9}" type="CELLRANGE">
+                    <a:fld id="{6771CC90-60C1-49AC-B682-445532628314}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[INTERVALLOCELLE]</a:t>
@@ -1302,7 +1303,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4C3D0221-6F7B-4BCC-86CE-E894E5A2468C}" type="CELLRANGE">
+                    <a:fld id="{33163958-4F79-4A82-853A-DB94D2BC8101}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[INTERVALLOCELLE]</a:t>
@@ -1334,8 +1335,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{29BB0969-50BD-4BD4-A657-4CD839DE397B}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{E6CB752A-581E-4A6F-A537-EF521EEC6AD1}" type="CELLRANGE">
+                      <a:rPr lang="it-IT"/>
                       <a:pPr/>
                       <a:t>[INTERVALLOCELLE]</a:t>
                     </a:fld>
@@ -1352,6 +1353,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -1366,8 +1368,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1D9CCAC9-22BE-4077-8A46-904539B98AE4}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{8B6C7F64-0C49-4753-B373-39D09147E91D}" type="CELLRANGE">
+                      <a:rPr lang="it-IT"/>
                       <a:pPr/>
                       <a:t>[INTERVALLOCELLE]</a:t>
                     </a:fld>
@@ -1384,6 +1386,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -1628,7 +1631,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B741A581-ADD3-4F82-90D5-691A91532904}" type="CELLRANGE">
+                    <a:fld id="{EDE52F76-C30F-497A-BF76-7B932A5694F7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[INTERVALLOCELLE]</a:t>
@@ -1667,7 +1670,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8871AB94-867B-4C7C-B5B7-44AB48FDB621}" type="CELLRANGE">
+                    <a:fld id="{F4FC7223-5F3C-4D7E-A1D9-3C51EEEA73A5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[INTERVALLOCELLE]</a:t>
@@ -1706,7 +1709,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2A39801D-91A3-4F5B-9C10-937D3D62B466}" type="CELLRANGE">
+                    <a:fld id="{8CF4237E-9B03-4F14-951E-376E761C404D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[INTERVALLOCELLE]</a:t>
@@ -1897,6 +1900,189 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{87A39A56-73B7-44F8-B95B-D219A00C2BDC}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[INTERVALLOCELLE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="it-IT"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-1887-4248-A1E7-E91D894DAB28}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-8.6132632588980101E-3"/>
+                  <c:y val="-7.0921999017516243E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{37F88443-A2BD-4838-9262-D65C3AE918C1}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[INTERVALLOCELLE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="it-IT"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-1887-4248-A1E7-E91D894DAB28}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-1887-4248-A1E7-E91D894DAB28}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-1887-4248-A1E7-E91D894DAB28}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="it-IT"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showDataLabelsRange val="1"/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:xVal>
             <c:numRef>
               <c:f>(Result!$D$15:$D$16,Result!$F$15:$F$16)</c:f>
@@ -1941,6 +2127,17 @@
           </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:datalabelsRange>
+                <c15:f>(Result!$B$18,Result!$B$16)</c15:f>
+                <c15:dlblRangeCache>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="1">
+                    <c:v>S7</c:v>
+                  </c:pt>
+                </c15:dlblRangeCache>
+              </c15:datalabelsRange>
+            </c:ext>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000A-BBC6-4AA6-B983-D887573D0A23}"/>
             </c:ext>
@@ -3288,7 +3485,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z14" sqref="Z14"/>
+      <selection activeCell="Y14" sqref="Y14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>